<commit_message>
Update code list dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/grout_inj_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/grout_inj_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4307EB82-3615-D547-84AC-52D70A3F8985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432D3342-C9F1-2245-9B65-18636ABBEEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17320" yWindow="9700" windowWidth="35840" windowHeight="20900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22060" yWindow="3560" windowWidth="35840" windowHeight="20900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="346">
   <si>
     <t>Description</t>
   </si>
@@ -1058,26 +1058,29 @@
     <t>Rotational force of the drill</t>
   </si>
   <si>
-    <t>//diggs:GroutInjectionProperty/diggs:propertyClass</t>
-  </si>
-  <si>
-    <t>//diggs:ContinuousGroutInjectionProperty/diggs:propertyClass</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>propertyClass</t>
   </si>
   <si>
     <t>Dictionary defining the values for recorded grout injection properties for both staged and continuous grouting activities. These values are used in the propertyClass property of the "GroutinjectionProperty" and "ContinuousGroutInjectionProperty" objects.</t>
+  </si>
+  <si>
+    <t>Time instant of measurement</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>//diggs:GroutStage//diggs:propertyClass</t>
+  </si>
+  <si>
+    <t>//diggs:ContinuousGrouting//diggs:propertyClass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1170,8 +1173,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1190,8 +1206,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1245,6 +1267,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1259,7 +1296,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1305,6 +1342,32 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1320,6 +1383,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1451,10 +1518,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1539,37 +1602,38 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H36" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H37" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:H37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2866,1,FALSE)),"Not used","")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B872,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D43" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:D43" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:E45" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E45" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
     <sortCondition ref="C1:C2"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="2">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</calculatedColumnFormula>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement"/>
+    <tableColumn id="5" xr3:uid="{70DA9ABB-01EE-9C4D-9F26-0BFC80A8CC6E}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1898,7 +1962,7 @@
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>233</v>
@@ -1907,7 +1971,7 @@
         <v>234</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -1923,15 +1987,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="B8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="84.6640625" style="2" customWidth="1"/>
@@ -1970,7 +2034,7 @@
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2866,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B872,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B2" s="16" t="s">
@@ -1992,7 +2056,7 @@
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2867,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B873,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B3" s="16" t="s">
@@ -2014,7 +2078,7 @@
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B2868,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B874,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="16" t="s">
@@ -2036,7 +2100,7 @@
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2869,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B875,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B5" s="16" t="s">
@@ -2058,7 +2122,7 @@
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2870,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B876,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" s="16" t="s">
@@ -2080,7 +2144,7 @@
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B877,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" s="16" t="s">
@@ -2102,7 +2166,7 @@
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2872,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B878,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B8" s="16" t="s">
@@ -2124,7 +2188,7 @@
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B879,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B9" s="16" t="s">
@@ -2146,7 +2210,7 @@
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B880,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" s="16" t="s">
@@ -2168,7 +2232,7 @@
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2875,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B881,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" s="16" t="s">
@@ -2190,7 +2254,7 @@
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B882,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" s="16" t="s">
@@ -2212,7 +2276,7 @@
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B883,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B13" s="16" t="s">
@@ -2234,7 +2298,7 @@
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2878,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B884,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B14" s="16" t="s">
@@ -2256,7 +2320,7 @@
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2879,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B885,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B15" s="16" t="s">
@@ -2278,7 +2342,7 @@
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2880,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B886,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B16" s="16" t="s">
@@ -2300,7 +2364,7 @@
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2881,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B887,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B17" s="16" t="s">
@@ -2322,7 +2386,7 @@
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B2882,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B888,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B18" s="16" t="s">
@@ -2344,7 +2408,7 @@
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2883,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B889,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B19" s="16" t="s">
@@ -2366,7 +2430,7 @@
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2884,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B890,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B20" s="16" t="s">
@@ -2388,7 +2452,7 @@
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2885,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B891,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B21" s="16" t="s">
@@ -2410,7 +2474,7 @@
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2886,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B892,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B22" s="16" t="s">
@@ -2432,7 +2496,7 @@
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2887,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B893,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B23" s="16" t="s">
@@ -2454,7 +2518,7 @@
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2888,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B894,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B24" s="16" t="s">
@@ -2476,7 +2540,7 @@
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2889,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B895,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B25" s="16" t="s">
@@ -2498,7 +2562,7 @@
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2890,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B896,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B26" s="16" t="s">
@@ -2520,7 +2584,7 @@
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2891,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B897,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B27" s="16" t="s">
@@ -2542,7 +2606,7 @@
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2892,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B898,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B28" s="16" t="s">
@@ -2564,7 +2628,7 @@
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2893,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B899,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B29" s="16" t="s">
@@ -2586,7 +2650,7 @@
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2894,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B900,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B30" s="16" t="s">
@@ -2608,7 +2672,7 @@
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2895,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B901,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B31" s="16" t="s">
@@ -2630,7 +2694,7 @@
     </row>
     <row r="32" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2896,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B902,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B32" s="16" t="s">
@@ -2650,9 +2714,9 @@
       </c>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2897,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B903,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B33" s="16" t="s">
@@ -2672,9 +2736,9 @@
       </c>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2898,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B904,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B34" s="16" t="s">
@@ -2694,9 +2758,9 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2899,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B905,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B35" s="16" t="s">
@@ -2716,9 +2780,9 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2900,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B906,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B36" s="16" t="s">
@@ -2737,6 +2801,29 @@
         <v>111</v>
       </c>
       <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="str">
+        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B907,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2762,11 +2849,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2777,7 +2864,7 @@
     <col min="4" max="4" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -2790,635 +2877,538 @@
       <c r="D1" s="6" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B2" s="14" t="s">
         <v>235</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B3" s="14" t="s">
         <v>238</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B4" s="14" t="s">
         <v>241</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B5" s="14" t="s">
         <v>244</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B6" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B7" s="14" t="s">
         <v>249</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D7" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B8" s="14" t="s">
         <v>252</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B9" t="s">
         <v>255</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B10" t="s">
         <v>255</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B11" s="14" t="s">
         <v>258</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D11" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B12" s="14" t="s">
         <v>261</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D12" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B13" s="14" t="s">
         <v>264</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D13" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B14" s="14" t="s">
         <v>267</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D14" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B15" s="14" t="s">
         <v>270</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D15" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B16" s="14" t="s">
         <v>273</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D16" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B17" s="14" t="s">
         <v>276</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D17" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B18" s="14" t="s">
         <v>279</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D18" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B19" s="14" t="s">
         <v>279</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D19" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B20" s="14" t="s">
         <v>282</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D20" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B21" s="14" t="s">
         <v>282</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D21" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B22" s="14" t="s">
         <v>285</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D22" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B23" s="14" t="s">
         <v>285</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D23" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B24" s="14" t="s">
         <v>288</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D24" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B25" s="14" t="s">
         <v>288</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D25" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B26" s="14" t="s">
         <v>291</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B27" s="14" t="s">
         <v>294</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D27" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B28" s="14" t="s">
         <v>297</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D28" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B29" s="14" t="s">
         <v>300</v>
       </c>
       <c r="C29" t="s">
-        <v>340</v>
-      </c>
-      <c r="D29" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B30" s="14" t="s">
         <v>304</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D30" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B31" s="14" t="s">
         <v>307</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D31" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B32" s="14" t="s">
         <v>310</v>
       </c>
       <c r="C32" t="s">
-        <v>340</v>
-      </c>
-      <c r="D32" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B33" s="14" t="s">
         <v>314</v>
       </c>
       <c r="C33" t="s">
-        <v>340</v>
-      </c>
-      <c r="D33" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B34" s="14" t="s">
         <v>317</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D34" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B35" s="14" t="s">
         <v>320</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D35" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B36" s="14" t="s">
         <v>323</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D36" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B37" s="14" t="s">
         <v>326</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D37" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B38" s="14" t="s">
         <v>330</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D38" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B39" t="s">
         <v>330</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D39" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B40" t="s">
         <v>333</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="D40" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B41,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B41" t="s">
         <v>333</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D41" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B42,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B42" s="14" t="s">
         <v>336</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D42" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f>IF(ISNA(VLOOKUP(B43,Definitions!B$2:B$1846,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B43,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B43" s="14" t="s">
         <v>338</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D43" t="s">
-        <v>342</v>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="str">
+        <f>IF(ISNA(VLOOKUP(B44,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="28" t="str">
+        <f>IF(ISNA(VLOOKUP(B45,Definitions!B$2:B$1843,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>